<commit_message>
GoodInfo_v2 - 2021.11.18 尚未完成
</commit_message>
<xml_diff>
--- a/Filter_20211118.xlsx
+++ b/Filter_20211118.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaeon365-my.sharepoint.com/personal/raywu_aaeon_com_tw/Documents/_OLD/Documents/Python/TradingModel_GoodInfo_v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayWu\OneDrive - AAEON Technology\_OLD\Documents\Python\TradingModel_GoodInfo_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{FD168EEA-C151-47B3-9A95-410C09B09A0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B470A07F-4CE8-433F-A03D-F949241FC1DD}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{FD168EEA-C151-47B3-9A95-410C09B09A0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7D6DDABD-BA9E-4F1E-8699-F565FE2C5FB4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18816" windowHeight="7968" xr2:uid="{BB5F1CAA-E1B6-4EBE-A6F8-6173DC212885}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>代號</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>上海商銀</t>
+  </si>
+  <si>
+    <t>國票金</t>
   </si>
 </sst>
 </file>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B3AF64-E97A-4B17-84D4-7CC921E354DE}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52:C54"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1294,6 +1297,17 @@
         <v>75</v>
       </c>
       <c r="C54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>2889</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1308,12 +1322,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1526,15 +1537,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81046D84-71BA-4494-97FE-ABE61A155419}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1E403E-48E0-45A5-8A6B-E1BE8411359D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1559,18 +1582,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1E403E-48E0-45A5-8A6B-E1BE8411359D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81046D84-71BA-4494-97FE-ABE61A155419}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>